<commit_message>
Update from Github Action
</commit_message>
<xml_diff>
--- a/南京互联网公司统计汇总.xlsx
+++ b/南京互联网公司统计汇总.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,78 +521,74 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>南京耀多信息技术有限公司</t>
+          <t>南京叶子科技有限公司（南京OPPO）</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>江苏南京</t>
+          <t>xx区</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>技术部</t>
+          <t>xxx事业部</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Android</t>
+          <t>Java</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>9:00-18:00</t>
+          <t>9:00-18:30</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1h</t>
+          <t>1.5h</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>一开始996，后来发不起加班费不给加班了，欠的加班费也不发</t>
+          <t>135 加班，24 正常；大小周等等</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>最低额度</t>
+          <t>基数 xxxx，比例 xx%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>13薪还是根据公司业绩提供，是否折扣，折扣比例。</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>八折</t>
+          <t>是否打折，比如 xx%。</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>提供笔记本</t>
+          <t>工位大小，环境，是否提供设备，设备型号种类。</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>有</t>
+          <t>是否有入职就有，是否有前置条件才有。</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>钉钉位置打卡</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>老板阴晴不定，随意开除员工</t>
-        </is>
-      </c>
+          <t>是否严格打卡，使用的软件或者方式（比如钉钉或人脸识别）。</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2022-01-25 02:22:42</t>
+          <t>2022-01-25 03:43:17</t>
         </is>
       </c>
     </row>
@@ -602,74 +598,78 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>南京希音电子商务有限公司</t>
+          <t>南京耀多信息技术有限公司</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>天溯产业园</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>江苏南京</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>技术部</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>前端</t>
+          <t>Android</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10:00-18:00(到20:00有50补贴)</t>
+          <t>9:00-18:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>12:00-13:30</t>
+          <t>1h</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>看部门，不强制，有工时排名。</t>
+          <t>一开始996，后来发不起加班费不给加班了，欠的加班费也不发</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>基础工资的8%</t>
+          <t>最低额度</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>看部门盈利情况和个人绩效定</t>
+          <t>无</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>试用期6个月，100%工资不打折</t>
+          <t>八折</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>配mac m1+显示器，网吧工作环境，工位挤。</t>
+          <t>提供笔记本</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>法定年假，可用加班时长来调休</t>
+          <t>有</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>1月3次补卡</t>
+          <t>钉钉位置打卡</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>抠，舍得给校招生，不舍得给社招生。多余的调休时长换钱200/d</t>
+          <t>老板阴晴不定，随意开除员工</t>
         </is>
       </c>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2022-01-25 01:58:09</t>
+          <t>2022-01-25 02:22:42</t>
         </is>
       </c>
     </row>
@@ -679,78 +679,74 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>慧资环球</t>
+          <t>南京希音电子商务有限公司</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>白下（年中搬到河西）</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>研发中心</t>
-        </is>
-      </c>
+          <t>天溯产业园</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>.NET/Python etc.</t>
+          <t>前端</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>自己安排，满8小时工时就好</t>
+          <t>10:00-18:00(到20:00有50补贴)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>自己安排</t>
+          <t>12:00-13:30</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>不加班</t>
+          <t>看部门，不强制，有工时排名。</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>全额8%</t>
+          <t>基础工资的8%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>13薪，每年调薪一次</t>
+          <t>看部门盈利情况和个人绩效定</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>不打折</t>
+          <t>试用期6个月，100%工资不打折</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>一个高配台式机或者一个高配Dell工作站笔记本，两个40寸4K显示器 Processor Intel(R) Core(TM) i9-10980XE CPU @ 3.00GHz 3.00 GHz  128GB RAM (新的台式机配置标准)</t>
+          <t>配mac m1+显示器，网吧工作环境，工位挤。</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>10 ~ 20天</t>
+          <t>法定年假，可用加班时长来调休</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>完全不打卡</t>
+          <t>1月3次补卡</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>内推VX：Just1n</t>
+          <t>抠，舍得给校招生，不舍得给社招生。多余的调休时长换钱200/d</t>
         </is>
       </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2022-01-24 14:35:55</t>
+          <t>2022-01-25 01:58:09</t>
         </is>
       </c>
     </row>
@@ -760,28 +756,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>零字节</t>
+          <t>慧资环球</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>建邺</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>白下（年中搬到河西）</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>研发中心</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Go/Rust/JS/TS/产品/运营</t>
+          <t>.NET/Python etc.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>9：30-6：30</t>
+          <t>自己安排，满8小时工时就好</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1.5h</t>
+          <t>自己安排</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>8%</t>
+          <t>全额8%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -801,33 +801,33 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>应届生八折，有工作经验的不打折</t>
+          <t>不打折</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>macbook pro（入职满三年电脑转赠给员工），每人配一个显示器（24-32寸）</t>
+          <t>一个高配台式机或者一个高配Dell工作站笔记本，两个40寸4K显示器 Processor Intel(R) Core(TM) i9-10980XE CPU @ 3.00GHz 3.00 GHz  128GB RAM (新的台式机配置标准)</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>入职转正就享受年假</t>
+          <t>10 ~ 20天</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>飞书打卡</t>
+          <t>完全不打卡</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>节日红包、年度旅游（21年三亚一周）</t>
+          <t>内推VX：Just1n</t>
         </is>
       </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2022-01-24 14:32:45</t>
+          <t>2022-01-24 14:35:55</t>
         </is>
       </c>
     </row>
@@ -837,27 +837,23 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>南京力方科技有限公司(力方智充)</t>
+          <t>零字节</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>雨花台区软件谷科创城</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>技术部</t>
-        </is>
-      </c>
+          <t>建邺</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Java</t>
+          <t>Go/Rust/JS/TS/产品/运营</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>9:00-18:00</t>
+          <t>9：30-6：30</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -867,44 +863,48 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>124固定加班到9点</t>
+          <t>不加班</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>最低，双边合计512</t>
+          <t>8%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>13薪，每年调薪一次</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>三个月，打八折</t>
+          <t>应届生八折，有工作经验的不打折</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>网吧工位，自带电脑</t>
+          <t>macbook pro（入职满三年电脑转赠给员工），每人配一个显示器（24-32寸）</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>法定年假</t>
+          <t>入职转正就享受年假</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>严格打卡，迟打卡扣30，不打卡半天工资</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr"/>
+          <t>飞书打卡</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>节日红包、年度旅游（21年三亚一周）</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>2022-01-24 14:29:37</t>
+          <t>2022-01-24 14:32:45</t>
         </is>
       </c>
     </row>
@@ -914,17 +914,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>硅基智能</t>
+          <t>南京力方科技有限公司(力方智充)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>软件大道</t>
+          <t>雨花台区软件谷科创城</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>创新产品事业群</t>
+          <t>技术部</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>9:00-18:30</t>
+          <t>9:00-18:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -944,44 +944,44 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>没事到点走，部门氛围卷</t>
+          <t>124固定加班到9点</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>基数5500，比例10%</t>
+          <t>最低，双边合计512</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>13薪还是根据公司业绩提供，是否折扣，折扣比例。</t>
+          <t>无</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>不打折</t>
+          <t>三个月，打八折</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>网吧工位</t>
+          <t>网吧工位，自带电脑</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>满一年才有正常年假，年假次年一月发放（不满一年打折）</t>
+          <t>法定年假</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>是否严格打卡，使用的软件或者方式（比如钉钉或人脸识别）。</t>
+          <t>严格打卡，迟打卡扣30，不打卡半天工资</t>
         </is>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>2022-01-24 14:25:34</t>
+          <t>2022-01-24 14:29:37</t>
         </is>
       </c>
     </row>
@@ -991,15 +991,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>百家云</t>
+          <t>硅基智能</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>雨花台软件谷科创城</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>软件大道</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>创新产品事业群</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>Java</t>
@@ -1017,36 +1021,44 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>周1,2,4正常加班，不想加班也行</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+          <t>没事到点走，部门氛围卷</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>基数5500，比例10%</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>13薪还是根据公司业绩提供，是否折扣，折扣比例。</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>6个月不打折。</t>
+          <t>不打折</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>mac笔记本+小米曲面屏显示器</t>
+          <t>网吧工位</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>年假次年一月发放，每满一年+1天</t>
+          <t>满一年才有正常年假，年假次年一月发放（不满一年打折）</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>每个月有4次迟到补卡机会，早上9.15之前打卡不算迟到</t>
+          <t>是否严格打卡，使用的软件或者方式（比如钉钉或人脸识别）。</t>
         </is>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>2022-01-24 14:21:22</t>
+          <t>2022-01-24 14:25:34</t>
         </is>
       </c>
     </row>
@@ -1056,19 +1068,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>创维南京分公司</t>
+          <t>百家云</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>雨花云密城</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>web后台</t>
-        </is>
-      </c>
+          <t>雨花台软件谷科创城</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>Java</t>
@@ -1076,7 +1084,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>09:30</t>
+          <t>9:00-18:30</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1086,44 +1094,36 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>995</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>工资八折的10%</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>1个月工资</t>
-        </is>
-      </c>
+          <t>周1,2,4正常加班，不想加班也行</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t>不打折</t>
+          <t>6个月不打折。</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Windows电脑+dell显示器</t>
+          <t>mac笔记本+小米曲面屏显示器</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>法定年假</t>
+          <t>年假次年一月发放，每满一年+1天</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>弹性打卡</t>
+          <t>每个月有4次迟到补卡机会，早上9.15之前打卡不算迟到</t>
         </is>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2022-01-24 14:19:34</t>
+          <t>2022-01-24 14:21:22</t>
         </is>
       </c>
     </row>
@@ -1133,15 +1133,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>新视云</t>
+          <t>创维南京分公司</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>雨花台</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+          <t>雨花云密城</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>web后台</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>Java</t>
@@ -1149,54 +1153,54 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>9:00-17:30</t>
+          <t>09:30</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1h</t>
+          <t>1.5h</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>看部门，业务部门偶尔加班，技术支持部门基本不加班</t>
+          <t>995</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>基数5k，比例8%</t>
+          <t>工资八折的10%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>固定13薪</t>
+          <t>1个月工资</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>3年合同，试用期总共6个月，前三个月8折，后三个月全薪</t>
+          <t>不打折</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>配笔记本+显示器</t>
+          <t>Windows电脑+dell显示器</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>5天年假+5天带薪病假（入职自动折算当年年假）</t>
+          <t>法定年假</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>不打卡</t>
+          <t>弹性打卡</t>
         </is>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2022-01-24 14:17:01</t>
+          <t>2022-01-24 14:19:34</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1210,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>华为</t>
+          <t>新视云</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>华为南研所</t>
+          <t>雨花台</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1222,54 +1226,54 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>9:00</t>
+          <t>9:00-17:30</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>12:00-13:40</t>
+          <t>1h</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>看部门情况。好部门：124加班8：30，35正常下班,差部门：天天11点以后</t>
+          <t>看部门，业务部门偶尔加班，技术支持部门基本不加班</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>基础工资的5%</t>
+          <t>基数5k，比例8%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>看部门盈利情况和个人绩效定</t>
+          <t>固定13薪</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>试用期6个月，100%工资不打折</t>
+          <t>3年合同，试用期总共6个月，前三个月8折，后三个月全薪</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>配win台式机+双屏</t>
+          <t>配笔记本+显示器</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>没签奋斗协议的5天，但一般不给休，第二年可以换成钱。签了的自愿放弃年假了</t>
+          <t>5天年假+5天带薪病假（入职自动折算当年年假）</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>必须按时打卡</t>
+          <t>不打卡</t>
         </is>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>2022-01-24 14:17:32</t>
+          <t>2022-01-24 14:17:01</t>
         </is>
       </c>
     </row>
@@ -1279,12 +1283,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>满帮</t>
+          <t>华为</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>雨花区万博科技园</t>
+          <t>华为南研所</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1295,42 +1299,54 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>9:00-18:30</t>
+          <t>9:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1.5h</t>
+          <t>12:00-13:40</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>看部门，不强制， 周五基本不加，还有每月一天奋斗日（年底算工资）， 据说要取消了</t>
+          <t>看部门情况。好部门：124加班8：30，35正常下班,差部门：天天11点以后</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>全额8%</t>
+          <t>基础工资的5%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>上下半年绩效</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr"/>
+          <t>看部门盈利情况和个人绩效定</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>试用期6个月，100%工资不打折</t>
+        </is>
+      </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>联想</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
+          <t>配win台式机+双屏</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>没签奋斗协议的5天，但一般不给休，第二年可以换成钱。签了的自愿放弃年假了</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>必须按时打卡</t>
+        </is>
+      </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2022-01-24 14:10:47</t>
+          <t>2022-01-24 14:17:32</t>
         </is>
       </c>
     </row>
@@ -1340,19 +1356,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A示例xxx公司</t>
+          <t>满帮</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>xx区</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>xxx事业部</t>
-        </is>
-      </c>
+          <t>雨花区万博科技园</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
           <t>Java</t>
@@ -1370,42 +1382,107 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>135 加班，24 正常；大小周等等</t>
+          <t>看部门，不强制， 周五基本不加，还有每月一天奋斗日（年底算工资）， 据说要取消了</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>基数 xxxx，比例 xx%</t>
+          <t>全额8%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>13薪还是根据公司业绩提供，是否折扣，折扣比例。</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>是否打折，比如 xx%。</t>
-        </is>
-      </c>
+          <t>上下半年绩效</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>工位大小，环境，是否提供设备，设备型号种类。</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>是否有入职就有，是否有前置条件才有。</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>是否严格打卡，使用的软件或者方式（比如钉钉或人脸识别）。</t>
-        </is>
-      </c>
+          <t>联想</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
+        <is>
+          <t>2022-01-24 14:10:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>A示例xxx公司</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>xx区</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>xxx事业部</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Java</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>9:00-18:30</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1.5h</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>135 加班，24 正常；大小周等等</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>基数 xxxx，比例 xx%</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>13薪还是根据公司业绩提供，是否折扣，折扣比例。</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>是否打折，比如 xx%。</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>工位大小，环境，是否提供设备，设备型号种类。</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>是否有入职就有，是否有前置条件才有。</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>是否严格打卡，使用的软件或者方式（比如钉钉或人脸识别）。</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>2022-01-24 13:11:01</t>
         </is>

</xml_diff>